<commit_message>
Substituído o arquivo BD.xlsx com a nova versão
</commit_message>
<xml_diff>
--- a/BD.xlsx
+++ b/BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\processos01\Desktop\Projetos\1-Andamento\Chechklist qualidade\CheklistEq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A462BAC-E40F-437E-BD7A-38F134AD5BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1613113E-2D48-47D2-8FA3-6683E8AE8A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7950" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7950" uniqueCount="433">
   <si>
     <t>Nivel</t>
   </si>
@@ -1113,142 +1113,307 @@
     <t>Faiscamento interno do rebolo (girar em sentido anti-horário)</t>
   </si>
   <si>
-    <t>O suporte da bandeja coletora de resíduos foi testado no chassi?</t>
-  </si>
-  <si>
-    <t>A bandeja coletora de resíduos possui pinos para batentes?</t>
-  </si>
-  <si>
-    <t>Os usinados soldados tem acabamento livre de cordão de solda*</t>
-  </si>
-  <si>
-    <t>As soldas dos tubos possuem acabamento liso?*</t>
-  </si>
-  <si>
-    <t>A gaiola se encaixa uniformemente ao ser abaixada sobre a rampa? *</t>
-  </si>
-  <si>
-    <t>A correção vertical foi testada com régua e esquadro?*</t>
-  </si>
-  <si>
-    <t>As tampas estão livres de empenamento?</t>
-  </si>
-  <si>
-    <t>A tampa do golpe está ajustada?</t>
-  </si>
-  <si>
-    <t>A esteira foi testada no chassi?</t>
-  </si>
-  <si>
-    <t>O Articulador esticador possui pino e guia?</t>
-  </si>
-  <si>
-    <t>O Alinhamento do suporte da pinça foi testado com esquadro?</t>
-  </si>
-  <si>
-    <t>A IHM foi testada com a furação no chassi?</t>
-  </si>
-  <si>
-    <t>A bandeja coletora de resíduos foi testada no chassi?</t>
-  </si>
-  <si>
-    <t>As furações entre chapas estão concêntricas?</t>
-  </si>
-  <si>
-    <t>Os furos roscados estão com rosca ao longo de toda sua extensão?</t>
-  </si>
-  <si>
-    <t>Todos os furos estão circulares?</t>
-  </si>
-  <si>
-    <t>Todos os furos especificados em projeto foram realizados?</t>
-  </si>
-  <si>
-    <t>Todas as soldas estão livres de poros e trincas?</t>
-  </si>
-  <si>
-    <t>Todas as soldas estão estruturadas e uniformes?</t>
-  </si>
-  <si>
-    <t>Todas as soldas estão livres de oxidação por calor?</t>
-  </si>
-  <si>
-    <t>A granulometria do escovamento está uniforme em toda a peça?</t>
-  </si>
-  <si>
-    <t>A peça está livre de aranhados?</t>
-  </si>
-  <si>
-    <t>O lado escovado está correto?</t>
-  </si>
-  <si>
-    <t>O sentido escovado está correto?</t>
-  </si>
-  <si>
-    <t>As extremidades externas estão arredondadas?</t>
-  </si>
-  <si>
-    <t>Todas as extremidades estão livres de rebarbas?</t>
-  </si>
-  <si>
-    <t>Todas as extremidades estão livres de cantos vivos?</t>
-  </si>
-  <si>
-    <t>Toda a estrutura tem acabamento liso livre de cordão de solda?</t>
-  </si>
-  <si>
-    <t>Os suportes internos dos sensores estão soldados?</t>
-  </si>
-  <si>
-    <t>As soldas de reforço interno do golpe estão conformes?</t>
-  </si>
-  <si>
-    <t>Foi realizado o teste do eixo lado móvel?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Os “passa fios” foram soldados na chapa de reforço? </t>
-  </si>
-  <si>
-    <t>A parte interna e externa do anel do golpe tem acabamento liso?</t>
-  </si>
-  <si>
-    <t>A parte interna e externa do golpe tem acabamento liso?</t>
-  </si>
-  <si>
-    <t>A parte superior da rampa estriada recebeu acabamento referênte as soldas da parte inferior?</t>
-  </si>
-  <si>
-    <t>A rampa estriada foi testada com o esquadro?</t>
-  </si>
-  <si>
-    <t>Os fixadores da rampa estriada estão encaixando corretamente na chapa da rampa?</t>
-  </si>
-  <si>
-    <t>Os fixadores da rampa estriada estão conformes?</t>
-  </si>
-  <si>
-    <t>A rampa estriada está com fixadores alinhadas?</t>
-  </si>
-  <si>
-    <t>A rampa foi testado com o gabarito?</t>
-  </si>
-  <si>
-    <t>Os cordões de solda de reforço foram soldados na parte interna do painel?</t>
-  </si>
-  <si>
-    <t>Os suportes universais foram soldados corretamente?</t>
-  </si>
-  <si>
-    <t>As dobradiças da tampa do painel tem cordão de solda de 4mm?</t>
-  </si>
-  <si>
-    <t>Foi realizado o teste de empenamento da chapa lateral esquerda do painel com régua metálica?</t>
-  </si>
-  <si>
-    <t>O Painel possui furação de esgotamento?</t>
-  </si>
-  <si>
-    <t>As furações estão centralizadas em relação a fixadores e usinados?</t>
+    <t>Painel-Todas as extremidades estão livres de cantos vivos?</t>
+  </si>
+  <si>
+    <t>Painel-Todas as extremidades estão livres de rebarbas?</t>
+  </si>
+  <si>
+    <t>Painel-As extremidades externas estão arredondadas?</t>
+  </si>
+  <si>
+    <t>Painel-O sentido escovado está correto?</t>
+  </si>
+  <si>
+    <t>Painel-O lado escovado está correto?</t>
+  </si>
+  <si>
+    <t>Painel-A peça está livre de aranhados?</t>
+  </si>
+  <si>
+    <t>Painel-A granulometria do escovamento está uniforme em toda a peça?</t>
+  </si>
+  <si>
+    <t>Painel-Todas as soldas estão livres de oxidação por calor?</t>
+  </si>
+  <si>
+    <t>Painel-Todas as soldas estão estruturadas e uniformes?</t>
+  </si>
+  <si>
+    <t>Painel-Todas as soldas estão livres de poros e trincas?</t>
+  </si>
+  <si>
+    <t>Painel-Todos os furos especificados em projeto foram realizados?</t>
+  </si>
+  <si>
+    <t>Painel-Todos os furos estão circulares?</t>
+  </si>
+  <si>
+    <t>Painel-Os furos roscados estão com rosca ao longo de toda sua extensão?</t>
+  </si>
+  <si>
+    <t>Painel-As furações entre chapas estão concêntricas?</t>
+  </si>
+  <si>
+    <t>Painel-As furações estão centralizadas em relação a fixadores e usinados?</t>
+  </si>
+  <si>
+    <t>Painel-O Painel possui furação de esgotamento?</t>
+  </si>
+  <si>
+    <t>Painel-Foi realizado o teste de empenamento da chapa lateral esquerda do painel com régua metálica?</t>
+  </si>
+  <si>
+    <t>Painel-As dobradiças da tampa do painel tem cordão de solda de 4mm?</t>
+  </si>
+  <si>
+    <t>Painel-Os suportes universais foram soldados corretamente?</t>
+  </si>
+  <si>
+    <t>Painel-Os cordões de solda de reforço foram soldados na parte interna do painel?</t>
+  </si>
+  <si>
+    <t>Rampa-Todas as extremidades estão livres de cantos vivos?</t>
+  </si>
+  <si>
+    <t>Rampa-Todas as extremidades estão livres de rebarbas?</t>
+  </si>
+  <si>
+    <t>Rampa-As extremidades externas estão arredondadas?</t>
+  </si>
+  <si>
+    <t>Rampa-O sentido escovado está correto?</t>
+  </si>
+  <si>
+    <t>Rampa-O lado escovado está correto?</t>
+  </si>
+  <si>
+    <t>Rampa-A peça está livre de aranhados?</t>
+  </si>
+  <si>
+    <t>Rampa-A granulometria do escovamento está uniforme em toda a peça?</t>
+  </si>
+  <si>
+    <t>Rampa-Todas as soldas estão livres de oxidação por calor?</t>
+  </si>
+  <si>
+    <t>Rampa-Todas as soldas estão estruturadas e uniformes?</t>
+  </si>
+  <si>
+    <t>Rampa-Todas as soldas estão livres de poros e trincas?</t>
+  </si>
+  <si>
+    <t>Rampa-Todos os furos especificados em projeto foram realizados?</t>
+  </si>
+  <si>
+    <t>Rampa-Todos os furos estão circulares?</t>
+  </si>
+  <si>
+    <t>Rampa-Os furos roscados estão com rosca ao longo de toda sua extensão?</t>
+  </si>
+  <si>
+    <t>Rampa-As furações entre chapas estão concêntricas?</t>
+  </si>
+  <si>
+    <t>Rampa-A rampa foi testado com o gabarito?</t>
+  </si>
+  <si>
+    <t>Rampa-A rampa estriada está com fixadores alinhadas?</t>
+  </si>
+  <si>
+    <t>Rampa-Os fixadores da rampa estriada estão conformes?</t>
+  </si>
+  <si>
+    <t>Rampa-Os fixadores da rampa estriada estão encaixando corretamente na chapa da rampa?</t>
+  </si>
+  <si>
+    <t>Rampa-A rampa estriada foi testada com o esquadro?</t>
+  </si>
+  <si>
+    <t>Rampa-A parte superior da rampa estriada recebeu acabamento referênte as soldas da parte inferior?</t>
+  </si>
+  <si>
+    <t>Golpe-Todas as extremidades estão livres de cantos vivos?</t>
+  </si>
+  <si>
+    <t>Golpe-Todas as extremidades estão livres de rebarbas?</t>
+  </si>
+  <si>
+    <t>Golpe-As extremidades externas estão arredondadas?</t>
+  </si>
+  <si>
+    <t>Golpe-O sentido escovado está correto?</t>
+  </si>
+  <si>
+    <t>Golpe-O lado escovado está correto?</t>
+  </si>
+  <si>
+    <t>Golpe-A peça está livre de aranhados?</t>
+  </si>
+  <si>
+    <t>Golpe-A granulometria do escovamento está uniforme em toda a peça?</t>
+  </si>
+  <si>
+    <t>Golpe-Todas as soldas estão livres de oxidação por calor?</t>
+  </si>
+  <si>
+    <t>Golpe-Todas as soldas estão estruturadas e uniformes?</t>
+  </si>
+  <si>
+    <t>Golpe-Todas as soldas estão livres de poros e trincas?</t>
+  </si>
+  <si>
+    <t>Golpe-Todos os furos especificados em projeto foram realizados?</t>
+  </si>
+  <si>
+    <t>Golpe-Todos os furos estão circulares?</t>
+  </si>
+  <si>
+    <t>Golpe-Os furos roscados estão com rosca ao longo de toda sua extensão?</t>
+  </si>
+  <si>
+    <t>Golpe-A parte interna e externa do golpe tem acabamento liso?</t>
+  </si>
+  <si>
+    <t>Golpe-A parte interna e externa do anel do golpe tem acabamento liso?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golpe-Os “passa fios” foram soldados na chapa de reforço? </t>
+  </si>
+  <si>
+    <t>Golpe-Foi realizado o teste do eixo lado móvel?</t>
+  </si>
+  <si>
+    <t>Golpe-As soldas de reforço interno do golpe estão conformes?</t>
+  </si>
+  <si>
+    <t>Golpe-Os suportes internos dos sensores estão soldados?</t>
+  </si>
+  <si>
+    <t>INF-Todas as extremidades estão livres de cantos vivos?</t>
+  </si>
+  <si>
+    <t>INF-Todas as extremidades estão livres de rebarbas?</t>
+  </si>
+  <si>
+    <t>INF-As extremidades externas estão arredondadas?</t>
+  </si>
+  <si>
+    <t>INF-O sentido escovado está correto?</t>
+  </si>
+  <si>
+    <t>INF-O lado escovado está correto?</t>
+  </si>
+  <si>
+    <t>INF-A peça está livre de aranhados?</t>
+  </si>
+  <si>
+    <t>INF-A granulometria do escovamento está uniforme em toda a peça?</t>
+  </si>
+  <si>
+    <t>INF-Todas as soldas estão livres de oxidação por calor?</t>
+  </si>
+  <si>
+    <t>INF-Todas as soldas estão estruturadas e uniformes?</t>
+  </si>
+  <si>
+    <t>INF-Todas as soldas estão livres de poros e trincas?</t>
+  </si>
+  <si>
+    <t>INF-Todos os furos especificados em projeto foram realizados?</t>
+  </si>
+  <si>
+    <t>INF-Todos os furos estão circulares?</t>
+  </si>
+  <si>
+    <t>INF-Os furos roscados estão com rosca ao longo de toda sua extensão?</t>
+  </si>
+  <si>
+    <t>INF-As furações entre chapas estão concêntricas?</t>
+  </si>
+  <si>
+    <t>Acessórios-Toda a estrutura tem acabamento liso livre de cordão de solda?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todas as extremidades estão livres de cantos vivos?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todas as extremidades estão livres de rebarbas?</t>
+  </si>
+  <si>
+    <t>Acessórios--As extremidades externas estão arredondadas?</t>
+  </si>
+  <si>
+    <t>Acessórios-O sentido escovado está correto?</t>
+  </si>
+  <si>
+    <t>Acessórios-O lado escovado está correto?</t>
+  </si>
+  <si>
+    <t>Acessórios-A peça está livre de aranhados?</t>
+  </si>
+  <si>
+    <t>Acessórios-A granulometria do escovamento está uniforme em toda a peça?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todas as soldas estão livres de oxidação por calor?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todas as soldas estão estruturadas e uniformes?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todas as soldas estão livres de poros e trincas?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todos os furos especificados em projeto foram realizados?</t>
+  </si>
+  <si>
+    <t>Acessórios-Todos os furos estão circulares?</t>
+  </si>
+  <si>
+    <t>Acessórios-Os furos roscados estão com rosca ao longo de toda sua extensão?</t>
+  </si>
+  <si>
+    <t>Acessórios-As furações entre chapas estão concêntricas?</t>
+  </si>
+  <si>
+    <t>Acessórios-A bandeja coletora de resíduos foi testada no chassi?</t>
+  </si>
+  <si>
+    <t>Acessórios-A IHM foi testada com a furação no chassi?</t>
+  </si>
+  <si>
+    <t>Acessórios-O Alinhamento do suporte da pinça foi testado com esquadro?</t>
+  </si>
+  <si>
+    <t>Acessórios-O Articulador esticador possui pino e guia?</t>
+  </si>
+  <si>
+    <t>Acessórios-A esteira foi testada no chassi?</t>
+  </si>
+  <si>
+    <t>Acessórios-A tampa do golpe está ajustada?</t>
+  </si>
+  <si>
+    <t>Acessórios-As tampas estão livres de empenamento?</t>
+  </si>
+  <si>
+    <t>Acessórios-A correção vertical foi testada com régua e esquadro?*</t>
+  </si>
+  <si>
+    <t>Acessórios-A gaiola se encaixa uniformemente ao ser abaixada sobre a rampa? *</t>
+  </si>
+  <si>
+    <t>Acessórios-As soldas dos tubos possuem acabamento liso?*</t>
+  </si>
+  <si>
+    <t>Acessórios-Os usinados soldados tem acabamento livre de cordão de solda*</t>
+  </si>
+  <si>
+    <t>Acessórios-A bandeja coletora de resíduos possui pinos para batentes?</t>
+  </si>
+  <si>
+    <t>Acessórios-O suporte da bandeja coletora de resíduos foi testado no chassi?</t>
   </si>
 </sst>
 </file>
@@ -1391,6 +1556,23 @@
   </cellStyles>
   <dxfs count="89">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="5"/>
@@ -1509,22 +1691,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1840,41 +2006,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F05952C4-41D4-4232-812A-8F025E459ADC}" name="Tabela15" displayName="Tabela15" ref="A1:AI172" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A1:AI172" xr:uid="{1DFFE8DB-5FAD-46E0-BAF6-F71ABF371AB8}"/>
   <tableColumns count="35">
-    <tableColumn id="3" xr3:uid="{3FBF9A9B-B895-4D2E-880B-63D24A14532D}" name="Parâmetros" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{31FC8D81-581A-44EA-AEC3-4333A928C19F}" name="FT-170" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{0732F65D-3800-47AC-8198-CF1621EEE971}" name="FT-250" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{0D49EE40-5D2E-4D2E-8433-21C360DC09C5}" name="FT-250 P" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{F48B237F-BA8C-4934-BB99-D1A2BB1D2B58}" name="FT-250 SM" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{F3DE9FD9-BA1F-47DB-BAF0-0EFA1BEA3000}" name="FTI-250 SM" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{EBE5D3C0-E269-45DC-B99A-83D1244CC06D}" name="FT-250 PLUS (Pinça Manual)" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{44DE7C95-3AFC-4919-88D0-403496BA5721}" name="FT-250 PLUS (Pinça pneumática)" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{692E4D21-3215-44B4-9D44-7B53EE43ABEE}" name="FTI-250" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{3D1C4EDC-5B5D-4364-9652-2842D7EA51B0}" name="FTI-250 PLUS (Pinça Manual)" dataDxfId="28"/>
-    <tableColumn id="13" xr3:uid="{E77B9CE5-E72F-4F87-B68E-0DA577303563}" name="FTI-250 PLUS (Pinça Pneumática)" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{11EA73A0-EC23-46F2-9893-8909700E228F}" name="FT-600" dataDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{EBEB2770-1E4A-4874-B70B-AD8F9B0B1989}" name="FT-600 AUT." dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{069FF7AE-7222-4486-9098-F69EAB0CC6A5}" name="FT-600 PLUS AUT." dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{61B4657D-B8DA-437E-9D4B-0DC8C4898D05}" name="FTI-600" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{95933D2D-F28B-46E9-9814-08F762D8E7EA}" name="FTI-600 AUT." dataDxfId="22"/>
-    <tableColumn id="19" xr3:uid="{8CB50DD0-C44C-4BCC-8253-0E1C82A5AE9F}" name="FTI-600 PLUS AUT." dataDxfId="21"/>
-    <tableColumn id="20" xr3:uid="{2A98D207-D910-40D2-B0D2-A9723CD577A1}" name="ST-250" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{7F47270B-C2C8-4C7A-A746-28B724F9CE0C}" name="ST-250 PLUS" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{D6C3361C-FD9D-4F57-86C7-64994FB8D8E9}" name="ST-250 EP" dataDxfId="18"/>
-    <tableColumn id="23" xr3:uid="{DF19851D-AEFC-497D-BCB9-11EA6E883328}" name="ST-300" dataDxfId="17"/>
-    <tableColumn id="24" xr3:uid="{78465341-68B3-4F21-AB4D-D9B6DFC640BB}" name="ST-300 AUT" dataDxfId="16"/>
-    <tableColumn id="25" xr3:uid="{86C7CC39-5394-4C7F-BF16-BFBF7AD52D3C}" name="ST-300 PLUS AUT" dataDxfId="15"/>
-    <tableColumn id="26" xr3:uid="{83BEE63E-3137-4A82-B77B-4476D92B813B}" name="STI-300 AUT" dataDxfId="14"/>
-    <tableColumn id="27" xr3:uid="{9232B313-1A1D-4F75-AA61-AC8F48F095FE}" name="STI-300 PLUS AUT" dataDxfId="13"/>
-    <tableColumn id="28" xr3:uid="{3AA6AD01-43F1-4251-9D44-BEE1A994454A}" name="SL-300 EP" dataDxfId="12"/>
-    <tableColumn id="29" xr3:uid="{5AC442DC-3605-481D-9D9D-4F344F689B19}" name="SL-300 PLUS EP" dataDxfId="11"/>
-    <tableColumn id="30" xr3:uid="{854DF0E5-5268-4C14-A249-2202105BA4A9}" name="SLI-300 EP" dataDxfId="10"/>
-    <tableColumn id="31" xr3:uid="{26A74F1A-39CE-4771-B996-FCBE4D7DF047}" name="SLI-300 PLUS EP" dataDxfId="9"/>
-    <tableColumn id="32" xr3:uid="{7377D182-E4EE-4926-AD1D-719CA5A562F3}" name="SL-300" dataDxfId="8"/>
-    <tableColumn id="33" xr3:uid="{CC77B1DA-05E9-40E7-ADFF-ACAF65FCE7EB}" name="SL-300 PLUS" dataDxfId="7"/>
-    <tableColumn id="34" xr3:uid="{1112DDEB-044A-4AD2-B305-701FB68D7C9F}" name="SLI-300" dataDxfId="6"/>
-    <tableColumn id="35" xr3:uid="{EC36CC51-4FDB-4E14-8D77-B2EA52682302}" name="SLI-300 PLUS" dataDxfId="5"/>
-    <tableColumn id="38" xr3:uid="{B25D6361-97E6-414B-97E5-2A93AFFE0282}" name="SLI-300 EP AUT" dataDxfId="4"/>
-    <tableColumn id="39" xr3:uid="{06A74C88-A2D9-4BF1-AA9A-4F755966C356}" name="SLI-300 PLUS EP AUT" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{3FBF9A9B-B895-4D2E-880B-63D24A14532D}" name="Parâmetros" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{31FC8D81-581A-44EA-AEC3-4333A928C19F}" name="FT-170" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{0732F65D-3800-47AC-8198-CF1621EEE971}" name="FT-250" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{0D49EE40-5D2E-4D2E-8433-21C360DC09C5}" name="FT-250 P" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{F48B237F-BA8C-4934-BB99-D1A2BB1D2B58}" name="FT-250 SM" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{F3DE9FD9-BA1F-47DB-BAF0-0EFA1BEA3000}" name="FTI-250 SM" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{EBE5D3C0-E269-45DC-B99A-83D1244CC06D}" name="FT-250 PLUS (Pinça Manual)" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{44DE7C95-3AFC-4919-88D0-403496BA5721}" name="FT-250 PLUS (Pinça pneumática)" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{692E4D21-3215-44B4-9D44-7B53EE43ABEE}" name="FTI-250" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{3D1C4EDC-5B5D-4364-9652-2842D7EA51B0}" name="FTI-250 PLUS (Pinça Manual)" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{E77B9CE5-E72F-4F87-B68E-0DA577303563}" name="FTI-250 PLUS (Pinça Pneumática)" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{11EA73A0-EC23-46F2-9893-8909700E228F}" name="FT-600" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{EBEB2770-1E4A-4874-B70B-AD8F9B0B1989}" name="FT-600 AUT." dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{069FF7AE-7222-4486-9098-F69EAB0CC6A5}" name="FT-600 PLUS AUT." dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{61B4657D-B8DA-437E-9D4B-0DC8C4898D05}" name="FTI-600" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{95933D2D-F28B-46E9-9814-08F762D8E7EA}" name="FTI-600 AUT." dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{8CB50DD0-C44C-4BCC-8253-0E1C82A5AE9F}" name="FTI-600 PLUS AUT." dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{2A98D207-D910-40D2-B0D2-A9723CD577A1}" name="ST-250" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{7F47270B-C2C8-4C7A-A746-28B724F9CE0C}" name="ST-250 PLUS" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{D6C3361C-FD9D-4F57-86C7-64994FB8D8E9}" name="ST-250 EP" dataDxfId="20"/>
+    <tableColumn id="23" xr3:uid="{DF19851D-AEFC-497D-BCB9-11EA6E883328}" name="ST-300" dataDxfId="19"/>
+    <tableColumn id="24" xr3:uid="{78465341-68B3-4F21-AB4D-D9B6DFC640BB}" name="ST-300 AUT" dataDxfId="18"/>
+    <tableColumn id="25" xr3:uid="{86C7CC39-5394-4C7F-BF16-BFBF7AD52D3C}" name="ST-300 PLUS AUT" dataDxfId="17"/>
+    <tableColumn id="26" xr3:uid="{83BEE63E-3137-4A82-B77B-4476D92B813B}" name="STI-300 AUT" dataDxfId="16"/>
+    <tableColumn id="27" xr3:uid="{9232B313-1A1D-4F75-AA61-AC8F48F095FE}" name="STI-300 PLUS AUT" dataDxfId="15"/>
+    <tableColumn id="28" xr3:uid="{3AA6AD01-43F1-4251-9D44-BEE1A994454A}" name="SL-300 EP" dataDxfId="14"/>
+    <tableColumn id="29" xr3:uid="{5AC442DC-3605-481D-9D9D-4F344F689B19}" name="SL-300 PLUS EP" dataDxfId="13"/>
+    <tableColumn id="30" xr3:uid="{854DF0E5-5268-4C14-A249-2202105BA4A9}" name="SLI-300 EP" dataDxfId="12"/>
+    <tableColumn id="31" xr3:uid="{26A74F1A-39CE-4771-B996-FCBE4D7DF047}" name="SLI-300 PLUS EP" dataDxfId="11"/>
+    <tableColumn id="32" xr3:uid="{7377D182-E4EE-4926-AD1D-719CA5A562F3}" name="SL-300" dataDxfId="10"/>
+    <tableColumn id="33" xr3:uid="{CC77B1DA-05E9-40E7-ADFF-ACAF65FCE7EB}" name="SL-300 PLUS" dataDxfId="9"/>
+    <tableColumn id="34" xr3:uid="{1112DDEB-044A-4AD2-B305-701FB68D7C9F}" name="SLI-300" dataDxfId="8"/>
+    <tableColumn id="35" xr3:uid="{EC36CC51-4FDB-4E14-8D77-B2EA52682302}" name="SLI-300 PLUS" dataDxfId="7"/>
+    <tableColumn id="38" xr3:uid="{B25D6361-97E6-414B-97E5-2A93AFFE0282}" name="SLI-300 EP AUT" dataDxfId="6"/>
+    <tableColumn id="39" xr3:uid="{06A74C88-A2D9-4BF1-AA9A-4F755966C356}" name="SLI-300 PLUS EP AUT" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15993,7 +16159,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:AJ1">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
@@ -16484,7 +16650,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A40">
-    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -17929,13 +18095,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2129A785-100C-4D25-97A6-0A2633651C78}">
   <dimension ref="A1:AK166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="2" customWidth="1"/>
@@ -17974,7 +18140,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -18084,7 +18250,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>38</v>
@@ -18193,7 +18359,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>38</v>
@@ -18302,7 +18468,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>38</v>
@@ -18411,7 +18577,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>38</v>
@@ -18520,7 +18686,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>38</v>
@@ -18629,7 +18795,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>38</v>
@@ -18738,7 +18904,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>38</v>
@@ -18847,7 +19013,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>38</v>
@@ -18956,7 +19122,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>38</v>
@@ -19065,7 +19231,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>38</v>
@@ -19174,7 +19340,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>38</v>
@@ -19283,7 +19449,7 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>38</v>
@@ -19392,7 +19558,7 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>38</v>
@@ -19610,7 +19776,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>377</v>
+        <v>346</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>38</v>
@@ -19719,7 +19885,7 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>38</v>
@@ -19828,7 +19994,7 @@
     </row>
     <row r="18" spans="1:37" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="B18" s="15"/>
       <c r="Z18" s="2" t="s">
@@ -19866,7 +20032,7 @@
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>374</v>
+        <v>349</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>38</v>
@@ -19885,7 +20051,7 @@
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="Z20" s="2" t="s">
         <v>38</v>
@@ -19922,7 +20088,7 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>38</v>
@@ -19971,7 +20137,7 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>38</v>
@@ -20080,7 +20246,7 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>38</v>
@@ -20189,7 +20355,7 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>38</v>
@@ -20407,7 +20573,7 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>38</v>
@@ -20516,7 +20682,7 @@
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>38</v>
@@ -20625,7 +20791,7 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>38</v>
@@ -20734,7 +20900,7 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>38</v>
@@ -20843,7 +21009,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>38</v>
@@ -20952,7 +21118,7 @@
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>38</v>
@@ -21061,7 +21227,7 @@
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>38</v>
@@ -21170,7 +21336,7 @@
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>38</v>
@@ -21279,7 +21445,7 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>38</v>
@@ -21388,7 +21554,7 @@
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>38</v>
@@ -21497,7 +21663,7 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15" t="s">
@@ -21532,7 +21698,7 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15" t="s">
@@ -21567,7 +21733,7 @@
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15" t="s">
@@ -21602,7 +21768,7 @@
     </row>
     <row r="39" spans="1:37" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15" t="s">
@@ -21637,7 +21803,7 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15" t="s">
@@ -21672,7 +21838,7 @@
     </row>
     <row r="41" spans="1:37" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>38</v>
@@ -21706,7 +21872,7 @@
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>38</v>
@@ -21815,7 +21981,7 @@
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>357</v>
+        <v>373</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>38</v>
@@ -21924,7 +22090,7 @@
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>38</v>
@@ -22033,7 +22199,7 @@
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>38</v>
@@ -22142,7 +22308,7 @@
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>38</v>
@@ -22251,7 +22417,7 @@
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>38</v>
@@ -22360,7 +22526,7 @@
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>38</v>
@@ -22469,7 +22635,7 @@
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>351</v>
+        <v>379</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>38</v>
@@ -22578,7 +22744,7 @@
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>350</v>
+        <v>380</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>38</v>
@@ -22687,7 +22853,7 @@
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>349</v>
+        <v>381</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>38</v>
@@ -22796,7 +22962,7 @@
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>38</v>
@@ -22905,7 +23071,7 @@
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>347</v>
+        <v>383</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>38</v>
@@ -23014,7 +23180,7 @@
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>346</v>
+        <v>384</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>38</v>
@@ -23123,7 +23289,7 @@
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>38</v>
@@ -23232,7 +23398,7 @@
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>38</v>
@@ -23341,7 +23507,7 @@
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>38</v>
@@ -23447,7 +23613,7 @@
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>362</v>
+        <v>388</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>38</v>
@@ -23556,7 +23722,7 @@
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>361</v>
+        <v>389</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>38</v>
@@ -23665,7 +23831,7 @@
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>360</v>
+        <v>390</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>38</v>
@@ -23774,7 +23940,7 @@
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>358</v>
+        <v>391</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>38</v>
@@ -23883,7 +24049,7 @@
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>357</v>
+        <v>392</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>38</v>
@@ -23992,7 +24158,7 @@
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
-        <v>356</v>
+        <v>393</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>38</v>
@@ -24101,7 +24267,7 @@
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
-        <v>355</v>
+        <v>394</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>38</v>
@@ -24210,7 +24376,7 @@
     </row>
     <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>354</v>
+        <v>395</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>38</v>
@@ -24319,7 +24485,7 @@
     </row>
     <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>38</v>
@@ -24428,7 +24594,7 @@
     </row>
     <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>352</v>
+        <v>397</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>38</v>
@@ -24537,7 +24703,7 @@
     </row>
     <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>351</v>
+        <v>398</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>38</v>
@@ -24646,7 +24812,7 @@
     </row>
     <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>350</v>
+        <v>399</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>38</v>
@@ -24755,7 +24921,7 @@
     </row>
     <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>349</v>
+        <v>400</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>38</v>
@@ -24864,7 +25030,7 @@
     </row>
     <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>348</v>
+        <v>401</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>38</v>
@@ -24973,7 +25139,7 @@
     </row>
     <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>347</v>
+        <v>402</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>38</v>
@@ -25082,7 +25248,7 @@
     </row>
     <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>346</v>
+        <v>403</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>38</v>
@@ -25191,7 +25357,7 @@
     </row>
     <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>345</v>
+        <v>404</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>38</v>
@@ -25300,7 +25466,7 @@
     </row>
     <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>359</v>
+        <v>405</v>
       </c>
       <c r="R75" s="2" t="s">
         <v>38</v>
@@ -25361,7 +25527,7 @@
     </row>
     <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>358</v>
+        <v>406</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>38</v>
@@ -25470,7 +25636,7 @@
     </row>
     <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
-        <v>357</v>
+        <v>407</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>38</v>
@@ -25579,7 +25745,7 @@
     </row>
     <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>356</v>
+        <v>408</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>38</v>
@@ -25688,7 +25854,7 @@
     </row>
     <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>355</v>
+        <v>409</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>38</v>
@@ -25797,7 +25963,7 @@
     </row>
     <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
-        <v>354</v>
+        <v>410</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>38</v>
@@ -25906,7 +26072,7 @@
     </row>
     <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>353</v>
+        <v>411</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>38</v>
@@ -26015,7 +26181,7 @@
     </row>
     <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>352</v>
+        <v>412</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>38</v>
@@ -26124,7 +26290,7 @@
     </row>
     <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
-        <v>351</v>
+        <v>413</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>38</v>
@@ -26233,7 +26399,7 @@
     </row>
     <row r="84" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>350</v>
+        <v>414</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>38</v>
@@ -26342,7 +26508,7 @@
     </row>
     <row r="85" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>349</v>
+        <v>415</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>38</v>
@@ -26451,7 +26617,7 @@
     </row>
     <row r="86" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>348</v>
+        <v>416</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>38</v>
@@ -26560,7 +26726,7 @@
     </row>
     <row r="87" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>347</v>
+        <v>417</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>38</v>
@@ -26669,7 +26835,7 @@
     </row>
     <row r="88" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>346</v>
+        <v>418</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>38</v>
@@ -26778,7 +26944,7 @@
     </row>
     <row r="89" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>345</v>
+        <v>419</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>38</v>
@@ -26887,7 +27053,7 @@
     </row>
     <row r="90" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>344</v>
+        <v>420</v>
       </c>
       <c r="B90" s="15"/>
       <c r="C90" s="15" t="s">
@@ -26931,7 +27097,7 @@
     </row>
     <row r="91" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>343</v>
+        <v>421</v>
       </c>
       <c r="B91" s="15"/>
       <c r="C91" s="15" t="s">
@@ -26999,7 +27165,7 @@
     </row>
     <row r="92" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>342</v>
+        <v>422</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="15" t="s">
@@ -27064,7 +27230,7 @@
     </row>
     <row r="93" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>341</v>
+        <v>423</v>
       </c>
       <c r="B93" s="15" t="s">
         <v>38</v>
@@ -27113,7 +27279,7 @@
     </row>
     <row r="94" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>340</v>
+        <v>424</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>38</v>
@@ -27157,7 +27323,7 @@
     </row>
     <row r="95" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>339</v>
+        <v>425</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>38</v>
@@ -27230,7 +27396,7 @@
     </row>
     <row r="96" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>338</v>
+        <v>426</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>38</v>
@@ -27339,7 +27505,7 @@
     </row>
     <row r="97" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>337</v>
+        <v>427</v>
       </c>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
@@ -27382,7 +27548,7 @@
     </row>
     <row r="98" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>336</v>
+        <v>428</v>
       </c>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
@@ -27425,7 +27591,7 @@
     </row>
     <row r="99" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>335</v>
+        <v>429</v>
       </c>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
@@ -27468,7 +27634,7 @@
     </row>
     <row r="100" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>334</v>
+        <v>430</v>
       </c>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
@@ -27535,7 +27701,7 @@
     </row>
     <row r="101" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>333</v>
+        <v>431</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>38</v>
@@ -27554,7 +27720,7 @@
     </row>
     <row r="102" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>38</v>
@@ -27829,7 +27995,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:AI1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>